<commit_message>
Update the product catalog with the latest compatibility information
Replace outdated product data file with a corrected version in data/Product Data.xlsx.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: a7aa588d-1f80-42db-be63-c6c7b4920eb3
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/873c23c0-c18f-4e09-9f8d-38c5cb319996/de977d80-35d9-4d3e-be59-79ec7843b909.jpg
</commit_message>
<xml_diff>
--- a/attached_assets/Product Data_05_28_2025.xlsx
+++ b/attached_assets/Product Data_05_28_2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bathcraft-my.sharepoint.com/personal/olep00903843_maax_com/Documents/PythonScripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="391" documentId="11_BCFEBD4F73F15EB6C55EF89F1835901893D73E67" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ACFAA825-518D-414D-AF57-3054951C2360}"/>
+  <xr:revisionPtr revIDLastSave="404" documentId="11_BCFEBD4F73F15EB6C55EF89F1835901893D73E67" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FF1BA00F-46AE-4C3F-A367-5A3E7D67436A}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-2730" windowWidth="38640" windowHeight="21120" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Tub Doors'!$A$1:$N$36</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'Tub Screens'!$A$1:$M$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Tub Showers'!$A$1:$L$45</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Walls!$A$1:$M$34</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Walls!$A$1:$M$38</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7449" uniqueCount="1784">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7493" uniqueCount="1789">
   <si>
     <t>Unique ID</t>
   </si>
@@ -5408,6 +5408,21 @@
   </si>
   <si>
     <t>https://maax.com/</t>
+  </si>
+  <si>
+    <t>Lineversa 4836 - Subway</t>
+  </si>
+  <si>
+    <t>Lineversa</t>
+  </si>
+  <si>
+    <t>Lineversa 6036 - Subway</t>
+  </si>
+  <si>
+    <t>Lineversa 6036 - Vertical</t>
+  </si>
+  <si>
+    <t>Lineversa 4836 - Vertical</t>
   </si>
 </sst>
 </file>
@@ -25603,11 +25618,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <sheetPr codeName="Sheet5" filterMode="1"/>
-  <dimension ref="A1:M34"/>
+  <sheetPr codeName="Sheet5"/>
+  <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="P37" sqref="P37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -25669,7 +25684,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="2" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>107455</v>
       </c>
@@ -25710,7 +25725,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="3" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>107464</v>
       </c>
@@ -25751,7 +25766,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="4" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>107458</v>
       </c>
@@ -25792,7 +25807,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="5" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>107456</v>
       </c>
@@ -25874,7 +25889,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="7" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>107457</v>
       </c>
@@ -25915,7 +25930,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="8" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>107466</v>
       </c>
@@ -26038,7 +26053,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="11" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>107460</v>
       </c>
@@ -26079,7 +26094,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="12" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>107479</v>
       </c>
@@ -26120,7 +26135,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="13" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>107352</v>
       </c>
@@ -26161,7 +26176,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="14" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>107461</v>
       </c>
@@ -26202,7 +26217,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="15" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>107462</v>
       </c>
@@ -26243,7 +26258,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="16" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>107228</v>
       </c>
@@ -26284,7 +26299,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="17" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>107465</v>
       </c>
@@ -26366,7 +26381,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="19" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>107459</v>
       </c>
@@ -26489,7 +26504,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="22" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>107227</v>
       </c>
@@ -26571,7 +26586,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="24" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>107224</v>
       </c>
@@ -26776,7 +26791,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="29" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>103388</v>
       </c>
@@ -26817,7 +26832,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="30" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>107463</v>
       </c>
@@ -26858,7 +26873,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="31" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>107223</v>
       </c>
@@ -26940,7 +26955,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="33" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>103378</v>
       </c>
@@ -27022,14 +27037,172 @@
         <v>1000</v>
       </c>
     </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
+        <v>182107</v>
+      </c>
+      <c r="B35" t="s">
+        <v>1784</v>
+      </c>
+      <c r="C35" t="s">
+        <v>1262</v>
+      </c>
+      <c r="D35" t="s">
+        <v>1783</v>
+      </c>
+      <c r="E35" t="s">
+        <v>35</v>
+      </c>
+      <c r="F35" t="s">
+        <v>700</v>
+      </c>
+      <c r="G35" t="s">
+        <v>706</v>
+      </c>
+      <c r="H35" t="s">
+        <v>702</v>
+      </c>
+      <c r="I35" t="s">
+        <v>711</v>
+      </c>
+      <c r="J35" t="s">
+        <v>19</v>
+      </c>
+      <c r="K35" t="s">
+        <v>20</v>
+      </c>
+      <c r="L35" t="s">
+        <v>1785</v>
+      </c>
+      <c r="M35">
+        <v>5010</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A36" s="1">
+        <v>180107</v>
+      </c>
+      <c r="B36" t="s">
+        <v>1786</v>
+      </c>
+      <c r="C36" t="s">
+        <v>1273</v>
+      </c>
+      <c r="D36" t="s">
+        <v>1783</v>
+      </c>
+      <c r="E36" t="s">
+        <v>43</v>
+      </c>
+      <c r="F36" t="s">
+        <v>642</v>
+      </c>
+      <c r="G36" t="s">
+        <v>706</v>
+      </c>
+      <c r="H36" t="s">
+        <v>702</v>
+      </c>
+      <c r="I36" t="s">
+        <v>711</v>
+      </c>
+      <c r="J36" t="s">
+        <v>19</v>
+      </c>
+      <c r="K36" t="s">
+        <v>20</v>
+      </c>
+      <c r="L36" t="s">
+        <v>1785</v>
+      </c>
+      <c r="M36">
+        <v>5010</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A37" s="1">
+        <v>181107</v>
+      </c>
+      <c r="B37" t="s">
+        <v>1787</v>
+      </c>
+      <c r="C37" t="s">
+        <v>1278</v>
+      </c>
+      <c r="D37" t="s">
+        <v>1783</v>
+      </c>
+      <c r="E37" t="s">
+        <v>43</v>
+      </c>
+      <c r="F37" t="s">
+        <v>642</v>
+      </c>
+      <c r="G37" t="s">
+        <v>706</v>
+      </c>
+      <c r="H37" t="s">
+        <v>702</v>
+      </c>
+      <c r="I37" t="s">
+        <v>711</v>
+      </c>
+      <c r="J37" t="s">
+        <v>19</v>
+      </c>
+      <c r="K37" t="s">
+        <v>20</v>
+      </c>
+      <c r="L37" t="s">
+        <v>1785</v>
+      </c>
+      <c r="M37">
+        <v>5010</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A38" s="1">
+        <v>183107</v>
+      </c>
+      <c r="B38" t="s">
+        <v>1788</v>
+      </c>
+      <c r="C38" t="s">
+        <v>1281</v>
+      </c>
+      <c r="D38" t="s">
+        <v>1783</v>
+      </c>
+      <c r="E38" t="s">
+        <v>35</v>
+      </c>
+      <c r="F38" t="s">
+        <v>700</v>
+      </c>
+      <c r="G38" t="s">
+        <v>706</v>
+      </c>
+      <c r="H38" t="s">
+        <v>702</v>
+      </c>
+      <c r="I38" t="s">
+        <v>711</v>
+      </c>
+      <c r="J38" t="s">
+        <v>19</v>
+      </c>
+      <c r="K38" t="s">
+        <v>20</v>
+      </c>
+      <c r="L38" t="s">
+        <v>1785</v>
+      </c>
+      <c r="M38">
+        <v>5010</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:M34" xr:uid="{00000000-0009-0000-0000-000004000000}">
-    <filterColumn colId="7">
-      <filters>
-        <filter val="Tub Wall Kit"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:M38" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
   <hyperlinks>
     <hyperlink ref="C17" r:id="rId1" xr:uid="{8BE85DCA-83E9-4797-8D4C-27CA93E39493}"/>
   </hyperlinks>

</xml_diff>

<commit_message>
Update product compatibility rules and data for better matching accuracy
Updates the product compatibility algorithm and data to enhance matching precision.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: a7aa588d-1f80-42db-be63-c6c7b4920eb3
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/873c23c0-c18f-4e09-9f8d-38c5cb319996/bc8b9553-d739-431e-9786-9193903a1d67.jpg
</commit_message>
<xml_diff>
--- a/attached_assets/Product Data_05_28_2025.xlsx
+++ b/attached_assets/Product Data_05_28_2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bathcraft-my.sharepoint.com/personal/olep00903843_maax_com/Documents/PythonScripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="404" documentId="11_BCFEBD4F73F15EB6C55EF89F1835901893D73E67" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FF1BA00F-46AE-4C3F-A367-5A3E7D67436A}"/>
+  <xr:revisionPtr revIDLastSave="430" documentId="11_BCFEBD4F73F15EB6C55EF89F1835901893D73E67" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{08E95847-07C9-4CEE-82AB-DAFD93ED6E46}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-2730" windowWidth="38640" windowHeight="21120" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7493" uniqueCount="1789">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7589" uniqueCount="1807">
   <si>
     <t>Unique ID</t>
   </si>
@@ -5423,6 +5423,60 @@
   </si>
   <si>
     <t>Lineversa 4836 - Vertical</t>
+  </si>
+  <si>
+    <t>TubVersaline</t>
+  </si>
+  <si>
+    <t>TubLineversa</t>
+  </si>
+  <si>
+    <t>107182-Tub</t>
+  </si>
+  <si>
+    <t>107180-Tub</t>
+  </si>
+  <si>
+    <t>107181-Tub</t>
+  </si>
+  <si>
+    <t>107183-Tub</t>
+  </si>
+  <si>
+    <t>182107-Tub</t>
+  </si>
+  <si>
+    <t>180107-Tub</t>
+  </si>
+  <si>
+    <t>181107-Tub</t>
+  </si>
+  <si>
+    <t>183107-Tub</t>
+  </si>
+  <si>
+    <t>Tub Versaline 4836 - Subway</t>
+  </si>
+  <si>
+    <t>Tub Versaline 6036 - Subway</t>
+  </si>
+  <si>
+    <t>Tub Versaline 6036 - Vertical</t>
+  </si>
+  <si>
+    <t>Tub Versaline 4836 - Vertical</t>
+  </si>
+  <si>
+    <t>Tub Lineversa 4836 - Subway</t>
+  </si>
+  <si>
+    <t>Tub Lineversa 6036 - Subway</t>
+  </si>
+  <si>
+    <t>Tub Lineversa 6036 - Vertical</t>
+  </si>
+  <si>
+    <t>Tub Lineversa 4836 - Vertical</t>
   </si>
 </sst>
 </file>
@@ -5543,10 +5597,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -25618,11 +25668,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:M38"/>
+  <sheetPr codeName="Sheet5" filterMode="1"/>
+  <dimension ref="A1:M46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -25638,7 +25688,7 @@
     <col min="9" max="9" width="12.21875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8.21875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.109375" customWidth="1"/>
+    <col min="12" max="12" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10" customWidth="1"/>
     <col min="16" max="16" width="34.88671875" bestFit="1" customWidth="1"/>
   </cols>
@@ -25684,8 +25734,8 @@
         <v>698</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2">
+    <row r="2" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
         <v>107455</v>
       </c>
       <c r="B2" t="s">
@@ -25725,8 +25775,8 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3">
+    <row r="3" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
         <v>107464</v>
       </c>
       <c r="B3" t="s">
@@ -25766,8 +25816,8 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4">
+    <row r="4" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
         <v>107458</v>
       </c>
       <c r="B4" t="s">
@@ -25807,8 +25857,8 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5">
+    <row r="5" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
         <v>107456</v>
       </c>
       <c r="B5" t="s">
@@ -25849,7 +25899,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="A6" s="1">
         <v>107182</v>
       </c>
       <c r="B6" t="s">
@@ -25889,8 +25939,8 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7">
+    <row r="7" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
         <v>107457</v>
       </c>
       <c r="B7" t="s">
@@ -25930,8 +25980,8 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8">
+    <row r="8" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
         <v>107466</v>
       </c>
       <c r="B8" t="s">
@@ -25971,8 +26021,8 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9">
+    <row r="9" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
         <v>141427</v>
       </c>
       <c r="B9" t="s">
@@ -26012,8 +26062,8 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10">
+    <row r="10" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
         <v>141425</v>
       </c>
       <c r="B10" t="s">
@@ -26053,8 +26103,8 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11">
+    <row r="11" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
         <v>107460</v>
       </c>
       <c r="B11" t="s">
@@ -26094,8 +26144,8 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12">
+    <row r="12" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
         <v>107479</v>
       </c>
       <c r="B12" t="s">
@@ -26135,8 +26185,8 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13">
+    <row r="13" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
         <v>107352</v>
       </c>
       <c r="B13" t="s">
@@ -26176,8 +26226,8 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A14">
+    <row r="14" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
         <v>107461</v>
       </c>
       <c r="B14" t="s">
@@ -26217,8 +26267,8 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A15">
+    <row r="15" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
         <v>107462</v>
       </c>
       <c r="B15" t="s">
@@ -26258,8 +26308,8 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16">
+    <row r="16" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
         <v>107228</v>
       </c>
       <c r="B16" t="s">
@@ -26299,8 +26349,8 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A17">
+    <row r="17" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
         <v>107465</v>
       </c>
       <c r="B17" t="s">
@@ -26341,7 +26391,7 @@
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A18">
+      <c r="A18" s="1">
         <v>107180</v>
       </c>
       <c r="B18" t="s">
@@ -26381,8 +26431,8 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A19">
+    <row r="19" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
         <v>107459</v>
       </c>
       <c r="B19" t="s">
@@ -26422,8 +26472,8 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A20">
+    <row r="20" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
         <v>103408</v>
       </c>
       <c r="B20" t="s">
@@ -26463,8 +26513,8 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A21">
+    <row r="21" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
         <v>103418</v>
       </c>
       <c r="B21" t="s">
@@ -26504,8 +26554,8 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A22">
+    <row r="22" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
         <v>107227</v>
       </c>
       <c r="B22" t="s">
@@ -26546,7 +26596,7 @@
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A23">
+      <c r="A23" s="1">
         <v>107181</v>
       </c>
       <c r="B23" t="s">
@@ -26586,8 +26636,8 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A24">
+    <row r="24" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
         <v>107224</v>
       </c>
       <c r="B24" t="s">
@@ -26627,8 +26677,8 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A25">
+    <row r="25" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
         <v>103424</v>
       </c>
       <c r="B25" t="s">
@@ -26669,7 +26719,7 @@
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A26">
+      <c r="A26" s="1">
         <v>107183</v>
       </c>
       <c r="B26" t="s">
@@ -26709,8 +26759,8 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A27">
+    <row r="27" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
         <v>107144</v>
       </c>
       <c r="B27" t="s">
@@ -26750,8 +26800,8 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A28">
+    <row r="28" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
         <v>107140</v>
       </c>
       <c r="B28" t="s">
@@ -26791,8 +26841,8 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A29">
+    <row r="29" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
         <v>103388</v>
       </c>
       <c r="B29" t="s">
@@ -26832,8 +26882,8 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A30">
+    <row r="30" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
         <v>107463</v>
       </c>
       <c r="B30" t="s">
@@ -26873,8 +26923,8 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A31">
+    <row r="31" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
         <v>107223</v>
       </c>
       <c r="B31" t="s">
@@ -26914,8 +26964,8 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A32">
+    <row r="32" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="1">
         <v>106542</v>
       </c>
       <c r="B32" t="s">
@@ -26955,8 +27005,8 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A33">
+    <row r="33" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
         <v>103378</v>
       </c>
       <c r="B33" t="s">
@@ -26996,8 +27046,8 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A34">
+    <row r="34" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="1">
         <v>103414</v>
       </c>
       <c r="B34" t="s">
@@ -27201,8 +27251,343 @@
         <v>5010</v>
       </c>
     </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B39" t="s">
+        <v>1799</v>
+      </c>
+      <c r="C39" t="s">
+        <v>1262</v>
+      </c>
+      <c r="D39" t="s">
+        <v>1783</v>
+      </c>
+      <c r="E39" t="s">
+        <v>35</v>
+      </c>
+      <c r="F39" t="s">
+        <v>700</v>
+      </c>
+      <c r="G39" t="s">
+        <v>706</v>
+      </c>
+      <c r="H39" t="s">
+        <v>710</v>
+      </c>
+      <c r="I39" t="s">
+        <v>711</v>
+      </c>
+      <c r="J39" t="s">
+        <v>19</v>
+      </c>
+      <c r="K39" t="s">
+        <v>20</v>
+      </c>
+      <c r="L39" t="s">
+        <v>1789</v>
+      </c>
+      <c r="M39">
+        <v>1510</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>1792</v>
+      </c>
+      <c r="B40" t="s">
+        <v>1800</v>
+      </c>
+      <c r="C40" t="s">
+        <v>1273</v>
+      </c>
+      <c r="D40" t="s">
+        <v>1783</v>
+      </c>
+      <c r="E40" t="s">
+        <v>43</v>
+      </c>
+      <c r="F40" t="s">
+        <v>642</v>
+      </c>
+      <c r="G40" t="s">
+        <v>706</v>
+      </c>
+      <c r="H40" t="s">
+        <v>710</v>
+      </c>
+      <c r="I40" t="s">
+        <v>711</v>
+      </c>
+      <c r="J40" t="s">
+        <v>19</v>
+      </c>
+      <c r="K40" t="s">
+        <v>20</v>
+      </c>
+      <c r="L40" t="s">
+        <v>1789</v>
+      </c>
+      <c r="M40">
+        <v>1510</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>1793</v>
+      </c>
+      <c r="B41" t="s">
+        <v>1801</v>
+      </c>
+      <c r="C41" t="s">
+        <v>1278</v>
+      </c>
+      <c r="D41" t="s">
+        <v>1783</v>
+      </c>
+      <c r="E41" t="s">
+        <v>43</v>
+      </c>
+      <c r="F41" t="s">
+        <v>642</v>
+      </c>
+      <c r="G41" t="s">
+        <v>706</v>
+      </c>
+      <c r="H41" t="s">
+        <v>710</v>
+      </c>
+      <c r="I41" t="s">
+        <v>711</v>
+      </c>
+      <c r="J41" t="s">
+        <v>19</v>
+      </c>
+      <c r="K41" t="s">
+        <v>20</v>
+      </c>
+      <c r="L41" t="s">
+        <v>1789</v>
+      </c>
+      <c r="M41">
+        <v>1510</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>1794</v>
+      </c>
+      <c r="B42" t="s">
+        <v>1802</v>
+      </c>
+      <c r="C42" t="s">
+        <v>1281</v>
+      </c>
+      <c r="D42" t="s">
+        <v>1783</v>
+      </c>
+      <c r="E42" t="s">
+        <v>35</v>
+      </c>
+      <c r="F42" t="s">
+        <v>700</v>
+      </c>
+      <c r="G42" t="s">
+        <v>706</v>
+      </c>
+      <c r="H42" t="s">
+        <v>710</v>
+      </c>
+      <c r="I42" t="s">
+        <v>711</v>
+      </c>
+      <c r="J42" t="s">
+        <v>19</v>
+      </c>
+      <c r="K42" t="s">
+        <v>20</v>
+      </c>
+      <c r="L42" t="s">
+        <v>1789</v>
+      </c>
+      <c r="M42">
+        <v>1510</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>1795</v>
+      </c>
+      <c r="B43" t="s">
+        <v>1803</v>
+      </c>
+      <c r="C43" t="s">
+        <v>1262</v>
+      </c>
+      <c r="D43" t="s">
+        <v>1783</v>
+      </c>
+      <c r="E43" t="s">
+        <v>35</v>
+      </c>
+      <c r="F43" t="s">
+        <v>700</v>
+      </c>
+      <c r="G43" t="s">
+        <v>706</v>
+      </c>
+      <c r="H43" t="s">
+        <v>710</v>
+      </c>
+      <c r="I43" t="s">
+        <v>711</v>
+      </c>
+      <c r="J43" t="s">
+        <v>19</v>
+      </c>
+      <c r="K43" t="s">
+        <v>20</v>
+      </c>
+      <c r="L43" t="s">
+        <v>1790</v>
+      </c>
+      <c r="M43">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>1796</v>
+      </c>
+      <c r="B44" t="s">
+        <v>1804</v>
+      </c>
+      <c r="C44" t="s">
+        <v>1273</v>
+      </c>
+      <c r="D44" t="s">
+        <v>1783</v>
+      </c>
+      <c r="E44" t="s">
+        <v>43</v>
+      </c>
+      <c r="F44" t="s">
+        <v>642</v>
+      </c>
+      <c r="G44" t="s">
+        <v>706</v>
+      </c>
+      <c r="H44" t="s">
+        <v>710</v>
+      </c>
+      <c r="I44" t="s">
+        <v>711</v>
+      </c>
+      <c r="J44" t="s">
+        <v>19</v>
+      </c>
+      <c r="K44" t="s">
+        <v>20</v>
+      </c>
+      <c r="L44" t="s">
+        <v>1790</v>
+      </c>
+      <c r="M44">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>1797</v>
+      </c>
+      <c r="B45" t="s">
+        <v>1805</v>
+      </c>
+      <c r="C45" t="s">
+        <v>1278</v>
+      </c>
+      <c r="D45" t="s">
+        <v>1783</v>
+      </c>
+      <c r="E45" t="s">
+        <v>43</v>
+      </c>
+      <c r="F45" t="s">
+        <v>642</v>
+      </c>
+      <c r="G45" t="s">
+        <v>706</v>
+      </c>
+      <c r="H45" t="s">
+        <v>710</v>
+      </c>
+      <c r="I45" t="s">
+        <v>711</v>
+      </c>
+      <c r="J45" t="s">
+        <v>19</v>
+      </c>
+      <c r="K45" t="s">
+        <v>20</v>
+      </c>
+      <c r="L45" t="s">
+        <v>1790</v>
+      </c>
+      <c r="M45">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>1798</v>
+      </c>
+      <c r="B46" t="s">
+        <v>1806</v>
+      </c>
+      <c r="C46" t="s">
+        <v>1281</v>
+      </c>
+      <c r="D46" t="s">
+        <v>1783</v>
+      </c>
+      <c r="E46" t="s">
+        <v>35</v>
+      </c>
+      <c r="F46" t="s">
+        <v>700</v>
+      </c>
+      <c r="G46" t="s">
+        <v>706</v>
+      </c>
+      <c r="H46" t="s">
+        <v>710</v>
+      </c>
+      <c r="I46" t="s">
+        <v>711</v>
+      </c>
+      <c r="J46" t="s">
+        <v>19</v>
+      </c>
+      <c r="K46" t="s">
+        <v>20</v>
+      </c>
+      <c r="L46" t="s">
+        <v>1790</v>
+      </c>
+      <c r="M46">
+        <v>1015</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:M38" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
+  <autoFilter ref="A1:M38" xr:uid="{00000000-0009-0000-0000-000004000000}">
+    <filterColumn colId="11">
+      <filters>
+        <filter val="Lineversa"/>
+        <filter val="Versaline"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <hyperlinks>
     <hyperlink ref="C17" r:id="rId1" xr:uid="{8BE85DCA-83E9-4797-8D4C-27CA93E39493}"/>
   </hyperlinks>

</xml_diff>